<commit_message>
Updated Code to connect excel with object[]
</commit_message>
<xml_diff>
--- a/EmployeeManagementAutomation/TestData/orange-test-data.xlsx
+++ b/EmployeeManagementAutomation/TestData/orange-test-data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Username</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Time at Work</t>
+  </si>
+  <si>
+    <t>kim124</t>
   </si>
 </sst>
 </file>
@@ -380,10 +383,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD1048576"/>
+      <selection activeCell="A3" sqref="A3:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -421,6 +424,17 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>